<commit_message>
added sample test to retrieve entire sheet
</commit_message>
<xml_diff>
--- a/ExcelApache/TestDataFile.xlsx
+++ b/ExcelApache/TestDataFile.xlsx
@@ -8,7 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sample" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Demo" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t xml:space="preserve">Testcases</t>
+    <t xml:space="preserve">TestCases</t>
   </si>
   <si>
     <t xml:space="preserve">Data1</t>
@@ -178,7 +180,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -266,4 +268,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Extracted data from excel spreadsheet
</commit_message>
<xml_diff>
--- a/ExcelApache/TestDataFile.xlsx
+++ b/ExcelApache/TestDataFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">TestCases</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">sadnnjsrj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdfaghh</t>
   </si>
   <si>
     <t xml:space="preserve">dfgasge</t>
@@ -96,6 +93,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,12 +178,12 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -238,25 +236,25 @@
       <c r="B4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -288,7 +286,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -314,7 +312,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>